<commit_message>
first 50 problems, implemented and documented
</commit_message>
<xml_diff>
--- a/docs/problem_list.xlsx
+++ b/docs/problem_list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="149">
   <si>
     <t>topic</t>
   </si>
@@ -67,7 +67,7 @@
     <t>reversedX == x</t>
   </si>
   <si>
-    <t>math.cpp</t>
+    <t>__</t>
   </si>
   <si>
     <t>Matrix, Array</t>
@@ -130,15 +130,18 @@
     <t xml:space="preserve"> Ransom Note</t>
   </si>
   <si>
+    <t xml:space="preserve">{val: amount} erase  if amount is 0 </t>
+  </si>
+  <si>
+    <t>Valid Anagram</t>
+  </si>
+  <si>
+    <t>_____</t>
+  </si>
+  <si>
     <t>string.cpp</t>
   </si>
   <si>
-    <t>Valid Anagram</t>
-  </si>
-  <si>
-    <t>_____</t>
-  </si>
-  <si>
     <t xml:space="preserve">LinkedList </t>
   </si>
   <si>
@@ -196,9 +199,6 @@
     <t>Intersection of Two Arrays II</t>
   </si>
   <si>
-    <t xml:space="preserve">{val: amount} erase  if amount is 0 </t>
-  </si>
-  <si>
     <t>twoPointers.cpp, hashing.cpp</t>
   </si>
   <si>
@@ -286,7 +286,7 @@
     <t>check dfs , bfs, dfs iterative solutions</t>
   </si>
   <si>
-    <t>binarTree.cpp</t>
+    <t>binaryTree.cpp</t>
   </si>
   <si>
     <t xml:space="preserve"> Balanced Binary Tree</t>
@@ -329,6 +329,141 @@
   </si>
   <si>
     <t>lowestSoFar</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor of Binary Search Tree</t>
+  </si>
+  <si>
+    <t>if p and q are on differnet sides =&gt; found LCA</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t>bfs</t>
+  </si>
+  <si>
+    <t>Binary Tree Right Side View</t>
+  </si>
+  <si>
+    <t>Backtracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Subsets</t>
+  </si>
+  <si>
+    <t>have i =&gt; left, without i=&gt; right</t>
+  </si>
+  <si>
+    <t>backtracking.cpp</t>
+  </si>
+  <si>
+    <t>priorityQueue</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in a St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heap </t>
+  </si>
+  <si>
+    <t>priorityQueue.cpp</t>
+  </si>
+  <si>
+    <t>Last Stone Weight</t>
+  </si>
+  <si>
+    <t>___</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validate Binary Search Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rightBoundry and leftBoundry </t>
+  </si>
+  <si>
+    <t>K Closest Points to Origin</t>
+  </si>
+  <si>
+    <t>min heap {distance,{x,y}}</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>Implement Trie (Prefix Tree)</t>
+  </si>
+  <si>
+    <t>  unordered_map&lt;char, TrieNode *&gt; children;</t>
+  </si>
+  <si>
+    <t>tier.cpp</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>Number of Islands</t>
+  </si>
+  <si>
+    <t>check 4 neighbors, mark 0 if visited</t>
+  </si>
+  <si>
+    <t>graph.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clone Graph</t>
+  </si>
+  <si>
+    <t>  unordered_map&lt;Node *, Node *&gt; oldToNew;</t>
+  </si>
+  <si>
+    <t>Combination Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don't increment  i for left side </t>
+  </si>
+  <si>
+    <t>Max Area of Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">see 200 </t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+  </si>
+  <si>
+    <t>fibonaci</t>
+  </si>
+  <si>
+    <t>dynamic.cpp</t>
+  </si>
+  <si>
+    <t>Min Stack</t>
+  </si>
+  <si>
+    <t>stack of &lt;value, minValueSoFar&gt; items</t>
+  </si>
+  <si>
+    <t>Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort by given lambda </t>
+  </si>
+  <si>
+    <t>Copy List with Random Pointer</t>
+  </si>
+  <si>
+    <t>unordered_map&lt;Node *, Node *&gt; map</t>
+  </si>
+  <si>
+    <t>LRU Cache</t>
+  </si>
+  <si>
+    <t>doubleLinkedList</t>
   </si>
 </sst>
 </file>
@@ -341,7 +476,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +534,30 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -543,7 +702,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,12 +724,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.25"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -885,137 +1038,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1025,7 +1178,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1037,7 +1189,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1357,10 +1520,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1369,7 +1532,7 @@
     <col min="2" max="2" width="6.45454545454545" style="3" customWidth="1"/>
     <col min="3" max="3" width="36.8545454545455" style="3" customWidth="1"/>
     <col min="4" max="4" width="15.2818181818182" customWidth="1"/>
-    <col min="5" max="5" width="18.6363636363636" customWidth="1"/>
+    <col min="5" max="5" width="46.3636363636364" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="6.14545454545455" customWidth="1"/>
     <col min="8" max="8" width="15.6363636363636" customWidth="1"/>
@@ -1414,22 +1577,22 @@
       </c>
     </row>
     <row r="2" ht="17" spans="1:8">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>45135</v>
       </c>
       <c r="G2">
@@ -1440,7 +1603,7 @@
       </c>
     </row>
     <row r="3" ht="17" spans="1:8">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="3">
@@ -1449,13 +1612,13 @@
       <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>45142</v>
       </c>
       <c r="G3">
@@ -1475,13 +1638,13 @@
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>45142</v>
       </c>
       <c r="G4">
@@ -1495,19 +1658,19 @@
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>387</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>45143</v>
       </c>
       <c r="G5">
@@ -1527,13 +1690,13 @@
       <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>45143</v>
       </c>
       <c r="G6">
@@ -1553,13 +1716,13 @@
       <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>45143</v>
       </c>
       <c r="G7">
@@ -1579,169 +1742,169 @@
       <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="8">
+        <v>37</v>
+      </c>
+      <c r="F8" s="7">
         <v>45144</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" ht="17" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>242</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>45144</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" ht="17" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3">
         <v>206</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="8">
+        <v>43</v>
+      </c>
+      <c r="F10" s="7">
         <v>45144</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" ht="17" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="10">
+        <v>41</v>
+      </c>
+      <c r="B11" s="9">
         <v>203</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="8">
+        <v>46</v>
+      </c>
+      <c r="F11" s="7">
         <v>45144</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" ht="17" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="10">
+        <v>41</v>
+      </c>
+      <c r="B12" s="9">
         <v>141</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="8">
+        <v>48</v>
+      </c>
+      <c r="F12" s="7">
         <v>45144</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" ht="17" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3">
         <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="8">
+        <v>50</v>
+      </c>
+      <c r="F13" s="7">
         <v>45144</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" ht="17" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="8">
+        <v>53</v>
+      </c>
+      <c r="F14" s="7">
         <v>45145</v>
       </c>
       <c r="G14">
@@ -1753,47 +1916,47 @@
     </row>
     <row r="15" ht="17" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B15" s="3">
         <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="8">
+        <v>56</v>
+      </c>
+      <c r="F15" s="7">
         <v>45145</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" ht="17" spans="1:8">
       <c r="A16" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B16" s="3">
         <v>350</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="8">
+        <v>37</v>
+      </c>
+      <c r="F16" s="7">
         <v>45145</v>
       </c>
       <c r="G16">
@@ -1805,7 +1968,7 @@
     </row>
     <row r="17" ht="17" spans="1:8">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3">
         <v>83</v>
@@ -1813,20 +1976,20 @@
       <c r="C17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E17" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <v>45145</v>
       </c>
       <c r="G17">
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" ht="17" spans="1:8">
@@ -1839,13 +2002,13 @@
       <c r="C18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E18" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="7">
         <v>45145</v>
       </c>
       <c r="G18">
@@ -1865,13 +2028,13 @@
       <c r="C19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E19" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="7">
         <v>45145</v>
       </c>
       <c r="G19">
@@ -1891,13 +2054,13 @@
       <c r="C20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E20" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <v>45145</v>
       </c>
       <c r="G20">
@@ -1909,7 +2072,7 @@
     </row>
     <row r="21" ht="17" spans="1:8">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B21" s="3">
         <v>232</v>
@@ -1917,25 +2080,25 @@
       <c r="C21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E21" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <v>45146</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="H21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" ht="17" spans="1:8">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B22" s="3">
         <v>2</v>
@@ -1943,20 +2106,20 @@
       <c r="C22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E22" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="7">
         <v>45148</v>
       </c>
       <c r="G22">
         <v>2</v>
       </c>
       <c r="H22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" ht="17" spans="1:8">
@@ -1969,13 +2132,13 @@
       <c r="C23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E23" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>45148</v>
       </c>
       <c r="G23">
@@ -1986,7 +2149,7 @@
       </c>
     </row>
     <row r="24" ht="17" spans="1:8">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>80</v>
       </c>
       <c r="B24" s="3">
@@ -1995,13 +2158,13 @@
       <c r="C24" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="7">
         <v>45148</v>
       </c>
       <c r="G24">
@@ -2015,19 +2178,19 @@
       <c r="A25" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>167</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E25" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <v>45149</v>
       </c>
       <c r="G25">
@@ -2047,13 +2210,13 @@
       <c r="C26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="7">
         <v>45150</v>
       </c>
       <c r="G26">
@@ -2073,13 +2236,13 @@
       <c r="C27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="7">
         <v>45152</v>
       </c>
       <c r="G27">
@@ -2099,13 +2262,13 @@
       <c r="C28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E28" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="7">
         <v>45152</v>
       </c>
       <c r="G28">
@@ -2125,13 +2288,13 @@
       <c r="C29" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <v>45152</v>
       </c>
       <c r="G29">
@@ -2145,19 +2308,19 @@
       <c r="A30" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>543</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="7">
         <v>45152</v>
       </c>
       <c r="G30">
@@ -2171,19 +2334,19 @@
       <c r="A31" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <v>572</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="7">
         <v>45152</v>
       </c>
       <c r="G31">
@@ -2195,7 +2358,7 @@
     </row>
     <row r="32" ht="17" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B32" s="3">
         <v>143</v>
@@ -2203,20 +2366,20 @@
       <c r="C32" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E32" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="7">
         <v>45153</v>
       </c>
       <c r="G32">
         <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" ht="17" spans="1:8">
@@ -2229,13 +2392,13 @@
       <c r="C33" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="7">
         <v>45159</v>
       </c>
       <c r="G33">
@@ -2245,12 +2408,486 @@
         <v>66</v>
       </c>
     </row>
+    <row r="34" ht="17.5" spans="1:8">
+      <c r="A34" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="14">
+        <v>235</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="7">
+        <v>45155</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" ht="17" spans="1:8">
+      <c r="A35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="3">
+        <v>102</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" t="s">
+        <v>107</v>
+      </c>
+      <c r="F35" s="7">
+        <v>45155</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" ht="17" spans="1:8">
+      <c r="A36" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="3">
+        <v>199</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" s="7">
+        <v>45156</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" ht="17" spans="1:8">
+      <c r="A37" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="3">
+        <v>78</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" s="7">
+        <v>45160</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" ht="17" spans="1:8">
+      <c r="A38" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="3">
+        <v>703</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="7">
+        <v>45162</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" ht="17" spans="1:8">
+      <c r="A39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1046</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s">
+        <v>118</v>
+      </c>
+      <c r="F39" s="7">
+        <v>45162</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" ht="17" spans="1:8">
+      <c r="A40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="17">
+        <v>98</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" s="7">
+        <v>45163</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" ht="17" spans="1:8">
+      <c r="A41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="3">
+        <v>973</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="F41" s="7">
+        <v>45163</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" ht="17" spans="1:8">
+      <c r="A42" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="3">
+        <v>208</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" s="7">
+        <v>45163</v>
+      </c>
+      <c r="G42">
+        <v>4</v>
+      </c>
+      <c r="H42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" ht="17" spans="1:8">
+      <c r="A43" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" s="3">
+        <v>200</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F43" s="7">
+        <v>45164</v>
+      </c>
+      <c r="G43">
+        <v>4</v>
+      </c>
+      <c r="H43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" ht="17" spans="1:8">
+      <c r="A44" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="3">
+        <v>133</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F44" s="7">
+        <v>45165</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" ht="17" spans="1:8">
+      <c r="A45" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" s="3">
+        <v>39</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" s="7">
+        <v>45165</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="H45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" ht="17" spans="1:8">
+      <c r="A46" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46" s="3">
+        <v>695</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" s="7">
+        <v>45165</v>
+      </c>
+      <c r="G46">
+        <v>4</v>
+      </c>
+      <c r="H46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" ht="17" spans="1:8">
+      <c r="A47" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" s="3">
+        <v>70</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" t="s">
+        <v>139</v>
+      </c>
+      <c r="F47" s="7">
+        <v>45166</v>
+      </c>
+      <c r="G47">
+        <v>5</v>
+      </c>
+      <c r="H47" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" ht="17" spans="1:8">
+      <c r="A48" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="3">
+        <v>155</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" t="s">
+        <v>142</v>
+      </c>
+      <c r="F48" s="7">
+        <v>45166</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" ht="17" spans="1:8">
+      <c r="A49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="3">
+        <v>347</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" t="s">
+        <v>144</v>
+      </c>
+      <c r="F49" s="7">
+        <v>45167</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" ht="17" spans="1:8">
+      <c r="A50" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="3">
+        <v>138</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F50" s="7">
+        <v>45167</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" ht="17" spans="1:8">
+      <c r="A51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="3">
+        <v>146</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" t="s">
+        <v>148</v>
+      </c>
+      <c r="F51" s="7">
+        <v>45167</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:L33">
+  <sortState ref="A2:L51">
     <sortCondition ref="F2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="Math" tooltip="https://leetcode.com/tag/math/"/>
+    <hyperlink ref="A37" r:id="rId2" display="Backtracking" tooltip="https://leetcode.com/tag/backtracking/"/>
+    <hyperlink ref="C42" r:id="rId3" display="Implement Trie (Prefix Tree)" tooltip="https://leetcode.com/problems/implement-trie-prefix-tree/"/>
+    <hyperlink ref="C43" r:id="rId4" display="Number of Islands" tooltip="https://leetcode.com/problems/number-of-islands/"/>
+    <hyperlink ref="C45" r:id="rId5" display="Combination Sum" tooltip="https://leetcode.com/problems/combination-sum/"/>
+    <hyperlink ref="C49" r:id="rId6" display="Top K Frequent Elements" tooltip="https://leetcode.com/problems/top-k-frequent-elements/"/>
+    <hyperlink ref="C51" r:id="rId7" display="LRU Cache" tooltip="https://leetcode.com/problems/lru-cache/"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait" horizontalDpi="600"/>

</xml_diff>